<commit_message>
- Deleted yellow and orange LEDs from design - Changed connector - Changed RESs and CAPs and used from our library - New layout - Changed polygon to thermal - Rearranged compenents in BOM
</commit_message>
<xml_diff>
--- a/Released/BOM/H09R01.xlsx
+++ b/Released/BOM/H09R01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Hexabitz\H09R0x-Hardware\Released\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D54EF0BE-154C-4E49-ADBA-5EA2320051F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{591F210B-F3AD-4E45-97FF-98630D3A1706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="-1395" windowWidth="21840" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15480" yWindow="-2670" windowWidth="15600" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="H09R0x" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="112">
   <si>
     <t>Description</t>
   </si>
@@ -190,9 +190,6 @@
     <t>C1</t>
   </si>
   <si>
-    <t>D3</t>
-  </si>
-  <si>
     <t>D1</t>
   </si>
   <si>
@@ -208,15 +205,6 @@
     <t>LED Uni-Color Super Red 639nm 2-Pin Chip 0603(1608Metric) T/R</t>
   </si>
   <si>
-    <t>D2</t>
-  </si>
-  <si>
-    <t>LED Uni-Color Soft Orange 611nm 2-Pin Chip 0603(1608Metric) T/R</t>
-  </si>
-  <si>
-    <t>https://octopart.com/vlmo1300-gs08-vishay-21709200?r=sp</t>
-  </si>
-  <si>
     <t>https://octopart.com/grm21bc81e475ka12l-murata-10331911?r=sp&amp;s=RY3qZSD8T6mG6TC9CHI5qQ</t>
   </si>
   <si>
@@ -253,15 +241,6 @@
     <t>Yageo</t>
   </si>
   <si>
-    <t>LED Uni-Color Soft Yellow 611nm 2-Pin Chip 0603(1608Metric) T/R</t>
-  </si>
-  <si>
-    <t>VLMY1300-GS08</t>
-  </si>
-  <si>
-    <t>https://octopart.com/vlmy1300-gs08-vishay-21709204?r=sp</t>
-  </si>
-  <si>
     <t>RC0603FR-07270RL</t>
   </si>
   <si>
@@ -322,12 +301,6 @@
     <t>CAP CER 0.01uF 50V X7R 0603</t>
   </si>
   <si>
-    <t>Wurth Elektronik</t>
-  </si>
-  <si>
-    <t>TERM BLOCK HDR 2POS VERT 5.08MM</t>
-  </si>
-  <si>
     <t>R4</t>
   </si>
   <si>
@@ -389,6 +362,15 @@
   </si>
   <si>
     <t>https://octopart.com/tlvh431acdbvr-texas+instruments-521919</t>
+  </si>
+  <si>
+    <t>Modular Terminal Block, 15A, 1 Row(s), 1 Deck(s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	1546111-2</t>
+  </si>
+  <si>
+    <t>https://octopart.com/1546111-2-te+connectivity+%2F+amp-40393356</t>
   </si>
 </sst>
 </file>
@@ -1028,10 +1010,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:G30"/>
+  <dimension ref="A2:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1104,7 +1086,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>14</v>
@@ -1176,7 +1158,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="17" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B11" s="17" t="s">
         <v>43</v>
@@ -1196,99 +1178,99 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="17" t="s">
-        <v>63</v>
+        <v>93</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E12" s="21" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="F12" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="F13" s="18">
         <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="E13" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="F13" s="18">
-        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="17" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E14" s="21" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="F14" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="17" t="s">
-        <v>102</v>
+        <v>77</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>104</v>
+        <v>38</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>103</v>
+        <v>62</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="E15" s="21" t="s">
-        <v>101</v>
+        <v>60</v>
       </c>
       <c r="F15" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="17" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E16" s="21" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F16" s="18">
         <v>1</v>
@@ -1296,39 +1278,39 @@
     </row>
     <row r="17" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="17" t="s">
-        <v>88</v>
+        <v>50</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>68</v>
+        <v>41</v>
       </c>
       <c r="E17" s="21" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="F17" s="18">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="17" t="s">
-        <v>50</v>
+        <v>82</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>39</v>
+        <v>78</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="E18" s="21" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="F18" s="18">
         <v>1</v>
@@ -1336,39 +1318,39 @@
     </row>
     <row r="19" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="17" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>85</v>
+        <v>37</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E19" s="21" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="F19" s="18">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="17" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="E20" s="21" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="F20" s="18">
         <v>1</v>
@@ -1379,7 +1361,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C21" s="17" t="s">
         <v>22</v>
@@ -1396,19 +1378,19 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="C22" s="17" t="s">
+      <c r="D22" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22" s="21" t="s">
         <v>53</v>
-      </c>
-      <c r="D22" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="E22" s="21" t="s">
-        <v>54</v>
       </c>
       <c r="F22" s="18">
         <v>1</v>
@@ -1416,59 +1398,59 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="17" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="C23" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="E23" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="D23" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="E23" s="21" t="s">
-        <v>59</v>
-      </c>
       <c r="F23" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="17" t="s">
-        <v>51</v>
+        <v>104</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>72</v>
+        <v>106</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>73</v>
+        <v>105</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>55</v>
+        <v>107</v>
       </c>
       <c r="E24" s="21" t="s">
-        <v>74</v>
+        <v>108</v>
       </c>
       <c r="F24" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="17" t="s">
-        <v>77</v>
+        <v>31</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>81</v>
+        <v>103</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>79</v>
+        <v>102</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>78</v>
+        <v>101</v>
       </c>
       <c r="E25" s="21" t="s">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="F25" s="18">
         <v>1</v>
@@ -1476,19 +1458,19 @@
     </row>
     <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="17" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>115</v>
+        <v>48</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>114</v>
+        <v>47</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>116</v>
+        <v>25</v>
       </c>
       <c r="E26" s="21" t="s">
-        <v>117</v>
+        <v>49</v>
       </c>
       <c r="F26" s="18">
         <v>1</v>
@@ -1496,19 +1478,19 @@
     </row>
     <row r="27" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="17" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C27" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="21" t="s">
         <v>111</v>
-      </c>
-      <c r="D27" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="E27" s="21" t="s">
-        <v>109</v>
       </c>
       <c r="F27" s="18">
         <v>1</v>
@@ -1516,59 +1498,21 @@
     </row>
     <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="17" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="E28" s="21" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="F28" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="B29" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="C29" s="17">
-        <v>691311500102</v>
-      </c>
-      <c r="D29" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="E29" s="21"/>
-      <c r="F29" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A30" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B30" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C30" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="D30" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="E30" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="F30" s="18">
         <v>1</v>
       </c>
     </row>
@@ -1580,29 +1524,27 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E21" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="E28" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="E30" r:id="rId3" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E26" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="E28" r:id="rId3" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
     <hyperlink ref="E10" r:id="rId4" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="E17" r:id="rId5" xr:uid="{01DF3B85-9108-476B-8AD5-F1F39BFC2F9F}"/>
-    <hyperlink ref="E13" r:id="rId6" xr:uid="{9CD624AB-68FA-45A0-BDA6-CACF754DD34A}"/>
-    <hyperlink ref="E18" r:id="rId7" xr:uid="{AE63E577-2AF8-4B24-A43D-F4255BA5FD41}"/>
+    <hyperlink ref="E19" r:id="rId5" xr:uid="{01DF3B85-9108-476B-8AD5-F1F39BFC2F9F}"/>
+    <hyperlink ref="E15" r:id="rId6" xr:uid="{9CD624AB-68FA-45A0-BDA6-CACF754DD34A}"/>
+    <hyperlink ref="E17" r:id="rId7" xr:uid="{AE63E577-2AF8-4B24-A43D-F4255BA5FD41}"/>
     <hyperlink ref="E11" r:id="rId8" xr:uid="{0A412581-708B-4B43-BCE9-F288010C1F6C}"/>
     <hyperlink ref="E22" r:id="rId9" xr:uid="{301AE570-2045-4255-B607-FD75AE5DA7F8}"/>
-    <hyperlink ref="E23" r:id="rId10" xr:uid="{AF654B3F-A2C7-4B2E-B564-D18FD2C0136B}"/>
-    <hyperlink ref="E19" r:id="rId11" xr:uid="{D0D8A6B6-6D38-4B73-B861-AACA1609CEF8}"/>
-    <hyperlink ref="E9" r:id="rId12" xr:uid="{48762FAB-6BA7-44F3-B66F-9D2208B135F2}"/>
-    <hyperlink ref="E12" r:id="rId13" xr:uid="{D2D372F9-DA4F-43C8-B46D-E866F10E6982}"/>
-    <hyperlink ref="E24" r:id="rId14" xr:uid="{210F0672-2960-4E6B-9F1A-CB6064DAE39D}"/>
-    <hyperlink ref="E25" r:id="rId15" xr:uid="{F4FAD961-1ACF-40F2-B70C-3F7C4560A218}"/>
-    <hyperlink ref="E20" r:id="rId16" xr:uid="{BE42E9FA-AD36-464F-AB3A-F7A444F116B6}"/>
-    <hyperlink ref="E14" r:id="rId17" xr:uid="{4AD7B685-7917-4523-AF44-27FA9A91852C}"/>
-    <hyperlink ref="E15" r:id="rId18" xr:uid="{533B9F78-9C0E-4DAA-B9A2-8296DDFD6413}"/>
-    <hyperlink ref="E16" r:id="rId19" xr:uid="{97A1D4CB-24CB-4CAF-A04F-E76BD7173ABB}"/>
-    <hyperlink ref="E27" r:id="rId20" xr:uid="{711190BD-4D14-40D2-A3FC-0F5868B01628}"/>
-    <hyperlink ref="E26" r:id="rId21" xr:uid="{D4B44AF4-2DFD-484D-A03C-C6F8A657311B}"/>
+    <hyperlink ref="E18" r:id="rId10" xr:uid="{D0D8A6B6-6D38-4B73-B861-AACA1609CEF8}"/>
+    <hyperlink ref="E9" r:id="rId11" xr:uid="{48762FAB-6BA7-44F3-B66F-9D2208B135F2}"/>
+    <hyperlink ref="E13" r:id="rId12" xr:uid="{D2D372F9-DA4F-43C8-B46D-E866F10E6982}"/>
+    <hyperlink ref="E23" r:id="rId13" xr:uid="{F4FAD961-1ACF-40F2-B70C-3F7C4560A218}"/>
+    <hyperlink ref="E20" r:id="rId14" xr:uid="{BE42E9FA-AD36-464F-AB3A-F7A444F116B6}"/>
+    <hyperlink ref="E14" r:id="rId15" xr:uid="{4AD7B685-7917-4523-AF44-27FA9A91852C}"/>
+    <hyperlink ref="E12" r:id="rId16" xr:uid="{533B9F78-9C0E-4DAA-B9A2-8296DDFD6413}"/>
+    <hyperlink ref="E16" r:id="rId17" xr:uid="{97A1D4CB-24CB-4CAF-A04F-E76BD7173ABB}"/>
+    <hyperlink ref="E25" r:id="rId18" xr:uid="{711190BD-4D14-40D2-A3FC-0F5868B01628}"/>
+    <hyperlink ref="E24" r:id="rId19" xr:uid="{D4B44AF4-2DFD-484D-A03C-C6F8A657311B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId22"/>
-  <drawing r:id="rId23"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId20"/>
+  <drawing r:id="rId21"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- Rearranged components in BOM
</commit_message>
<xml_diff>
--- a/Released/BOM/H09R01.xlsx
+++ b/Released/BOM/H09R01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Hexabitz\H09R0x-Hardware\Released\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{591F210B-F3AD-4E45-97FF-98630D3A1706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50779081-2D18-4294-AEC8-6D80BA2BDA44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-15480" yWindow="-2670" windowWidth="15600" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1013,7 +1013,7 @@
   <dimension ref="A2:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1278,19 +1278,19 @@
     </row>
     <row r="17" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="17" t="s">
-        <v>50</v>
+        <v>83</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>39</v>
+        <v>87</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>40</v>
+        <v>86</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="E17" s="21" t="s">
-        <v>42</v>
+        <v>84</v>
       </c>
       <c r="F17" s="18">
         <v>1</v>
@@ -1298,59 +1298,59 @@
     </row>
     <row r="18" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>78</v>
+        <v>37</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="E18" s="21" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="F18" s="18">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="17" t="s">
-        <v>81</v>
+        <v>50</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="E19" s="21" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="F19" s="18">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>86</v>
+        <v>58</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>85</v>
+        <v>57</v>
       </c>
       <c r="E20" s="21" t="s">
-        <v>84</v>
+        <v>56</v>
       </c>
       <c r="F20" s="18">
         <v>1</v>
@@ -1527,16 +1527,16 @@
     <hyperlink ref="E26" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
     <hyperlink ref="E28" r:id="rId3" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
     <hyperlink ref="E10" r:id="rId4" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="E19" r:id="rId5" xr:uid="{01DF3B85-9108-476B-8AD5-F1F39BFC2F9F}"/>
+    <hyperlink ref="E18" r:id="rId5" xr:uid="{01DF3B85-9108-476B-8AD5-F1F39BFC2F9F}"/>
     <hyperlink ref="E15" r:id="rId6" xr:uid="{9CD624AB-68FA-45A0-BDA6-CACF754DD34A}"/>
-    <hyperlink ref="E17" r:id="rId7" xr:uid="{AE63E577-2AF8-4B24-A43D-F4255BA5FD41}"/>
+    <hyperlink ref="E19" r:id="rId7" xr:uid="{AE63E577-2AF8-4B24-A43D-F4255BA5FD41}"/>
     <hyperlink ref="E11" r:id="rId8" xr:uid="{0A412581-708B-4B43-BCE9-F288010C1F6C}"/>
     <hyperlink ref="E22" r:id="rId9" xr:uid="{301AE570-2045-4255-B607-FD75AE5DA7F8}"/>
-    <hyperlink ref="E18" r:id="rId10" xr:uid="{D0D8A6B6-6D38-4B73-B861-AACA1609CEF8}"/>
+    <hyperlink ref="E20" r:id="rId10" xr:uid="{D0D8A6B6-6D38-4B73-B861-AACA1609CEF8}"/>
     <hyperlink ref="E9" r:id="rId11" xr:uid="{48762FAB-6BA7-44F3-B66F-9D2208B135F2}"/>
     <hyperlink ref="E13" r:id="rId12" xr:uid="{D2D372F9-DA4F-43C8-B46D-E866F10E6982}"/>
     <hyperlink ref="E23" r:id="rId13" xr:uid="{F4FAD961-1ACF-40F2-B70C-3F7C4560A218}"/>
-    <hyperlink ref="E20" r:id="rId14" xr:uid="{BE42E9FA-AD36-464F-AB3A-F7A444F116B6}"/>
+    <hyperlink ref="E17" r:id="rId14" xr:uid="{BE42E9FA-AD36-464F-AB3A-F7A444F116B6}"/>
     <hyperlink ref="E14" r:id="rId15" xr:uid="{4AD7B685-7917-4523-AF44-27FA9A91852C}"/>
     <hyperlink ref="E12" r:id="rId16" xr:uid="{533B9F78-9C0E-4DAA-B9A2-8296DDFD6413}"/>
     <hyperlink ref="E16" r:id="rId17" xr:uid="{97A1D4CB-24CB-4CAF-A04F-E76BD7173ABB}"/>

</xml_diff>

<commit_message>
- Changed logo in layout - Rearranged components in BOM
</commit_message>
<xml_diff>
--- a/Released/BOM/H09R01.xlsx
+++ b/Released/BOM/H09R01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Hexabitz\H09R0x-Hardware\Released\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50779081-2D18-4294-AEC8-6D80BA2BDA44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11BF409B-BD7D-4587-B64C-543A677FA3B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-15480" yWindow="-2670" windowWidth="15600" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1012,8 +1012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:XFD18"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1418,19 +1418,19 @@
     </row>
     <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="17" t="s">
-        <v>104</v>
+        <v>24</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>106</v>
+        <v>48</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>105</v>
+        <v>47</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>107</v>
+        <v>25</v>
       </c>
       <c r="E24" s="21" t="s">
-        <v>108</v>
+        <v>49</v>
       </c>
       <c r="F24" s="18">
         <v>1</v>
@@ -1458,19 +1458,19 @@
     </row>
     <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="17" t="s">
-        <v>24</v>
+        <v>104</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>48</v>
+        <v>106</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>47</v>
+        <v>105</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>25</v>
+        <v>107</v>
       </c>
       <c r="E26" s="21" t="s">
-        <v>49</v>
+        <v>108</v>
       </c>
       <c r="F26" s="18">
         <v>1</v>
@@ -1524,7 +1524,7 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E21" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="E26" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="E24" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
     <hyperlink ref="E28" r:id="rId3" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
     <hyperlink ref="E10" r:id="rId4" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
     <hyperlink ref="E18" r:id="rId5" xr:uid="{01DF3B85-9108-476B-8AD5-F1F39BFC2F9F}"/>
@@ -1541,7 +1541,7 @@
     <hyperlink ref="E12" r:id="rId16" xr:uid="{533B9F78-9C0E-4DAA-B9A2-8296DDFD6413}"/>
     <hyperlink ref="E16" r:id="rId17" xr:uid="{97A1D4CB-24CB-4CAF-A04F-E76BD7173ABB}"/>
     <hyperlink ref="E25" r:id="rId18" xr:uid="{711190BD-4D14-40D2-A3FC-0F5868B01628}"/>
-    <hyperlink ref="E24" r:id="rId19" xr:uid="{D4B44AF4-2DFD-484D-A03C-C6F8A657311B}"/>
+    <hyperlink ref="E26" r:id="rId19" xr:uid="{D4B44AF4-2DFD-484D-A03C-C6F8A657311B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId20"/>

</xml_diff>